<commit_message>
uploaded working pipeline with extra figure making scripts, and a Forrest_Wrapper to troubleshoot transprob problems
</commit_message>
<xml_diff>
--- a/Documents/Timestamps_video.xlsx
+++ b/Documents/Timestamps_video.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/judy/Video_HMM/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBA824E9-80AA-C840-BB86-AD18F05483C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B218AF2-7344-E14E-993D-6B1E8C7C27F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{B78C5E59-0D08-964B-90AA-CF643940375F}"/>
+    <workbookView xWindow="3300" yWindow="16780" windowWidth="28040" windowHeight="16940" xr2:uid="{B78C5E59-0D08-964B-90AA-CF643940375F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -160,7 +160,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -204,18 +204,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3310962-827B-AF4A-9BBC-5955E95DADE1}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,35 +560,35 @@
     <col min="7" max="7" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="9"/>
       <c r="H2" t="s">
         <v>31</v>
       </c>
@@ -597,7 +596,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -624,9 +623,8 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="L3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -653,9 +651,8 @@
         <f>J3+H3+$H$27</f>
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="L4" s="10"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -675,16 +672,15 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" ref="H4:H13" si="0">D5-C5</f>
+        <f t="shared" ref="H5:H12" si="0">D5-C5</f>
         <v>1.1111111111111112E-2</v>
       </c>
       <c r="J5" s="3">
         <f>J4+H4+$H$27</f>
         <v>2.8472222222222222E-2</v>
       </c>
-      <c r="L5" s="10"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -711,13 +707,12 @@
         <f>J5+H5+$H$27</f>
         <v>4.2361111111111113E-2</v>
       </c>
-      <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="4">
@@ -726,7 +721,7 @@
       <c r="D7" s="4">
         <v>1.4583333333333334E-2</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="8">
@@ -740,26 +735,24 @@
         <f>J6+H6+$H$27</f>
         <v>0.05</v>
       </c>
-      <c r="L7" s="10"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="4">
         <v>8.9583333333333334E-2</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="8"/>
       <c r="H8" s="3">
         <v>3.5416666666666666E-2</v>
       </c>
       <c r="J8" s="3"/>
-      <c r="L8" s="10"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -786,9 +779,8 @@
         <f>J7+H7+H8+$H$27</f>
         <v>9.0277777777777776E-2</v>
       </c>
-      <c r="L9" s="10"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -815,9 +807,8 @@
         <f>J9+H9+$H$27</f>
         <v>0.10138888888888889</v>
       </c>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -841,16 +832,15 @@
         <v>2.2916666666666665E-2</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" ref="J11:J12" si="1">J10+H10+$H$27</f>
+        <f t="shared" ref="J11" si="1">J10+H10+$H$27</f>
         <v>0.12777777777777777</v>
       </c>
-      <c r="L11" s="10"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="4">
@@ -859,7 +849,7 @@
       <c r="D12" s="4">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="8">
@@ -873,26 +863,24 @@
         <f>J11+H11+$H$27</f>
         <v>0.1534722222222222</v>
       </c>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
       <c r="C13" s="4">
         <v>4.7222222222222221E-2</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="8"/>
       <c r="H13" s="3">
         <v>1.8055555555555554E-2</v>
       </c>
       <c r="J13" s="3"/>
-      <c r="L13" s="10"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
         <v>38</v>
       </c>
@@ -900,9 +888,8 @@
         <f>J12+H12+H13</f>
         <v>0.18194444444444441</v>
       </c>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G15" t="s">
         <v>33</v>
       </c>

</xml_diff>